<commit_message>
Add conditional Probability to Prob_XY.xlsx
</commit_message>
<xml_diff>
--- a/Exam_prep/Prob_XY.xlsx
+++ b/Exam_prep/Prob_XY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Data Science\Risk Analysis\risk_analysis\Exam_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADB314C-43D6-42B7-9922-900D1F1307F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E1744B-A539-4021-B057-C4455CF86C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Enter your values here:</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>std(Y)</t>
+  </si>
+  <si>
+    <t>Conditional Probabilities:</t>
+  </si>
+  <si>
+    <t>P(Y|Z)</t>
+  </si>
+  <si>
+    <t>P(Z|Y)</t>
+  </si>
+  <si>
+    <t>E(Y|Z)</t>
+  </si>
+  <si>
+    <t>E(Z|Y)</t>
   </si>
 </sst>
 </file>
@@ -461,14 +476,32 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -477,24 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Anteckning" xfId="4" builtinId="10"/>
@@ -779,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:I24"/>
+  <dimension ref="A4:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B5" sqref="B5:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -790,32 +806,49 @@
     <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" customWidth="1"/>
+    <col min="19" max="19" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.453125" customWidth="1"/>
+    <col min="21" max="21" width="8.453125" customWidth="1"/>
+    <col min="22" max="22" width="9.26953125" customWidth="1"/>
+    <col min="23" max="23" width="9.6328125" customWidth="1"/>
+    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="K4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15">
-        <v>2</v>
-      </c>
-      <c r="E5" s="15">
-        <v>8</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="12" t="s">
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="T4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="20"/>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="15"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -824,27 +857,60 @@
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1">
+        <f>C$5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ref="N5:P5" si="0">D$5</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="1">
+        <f>C5</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:W5" si="1">D5</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21">
-        <v>0</v>
-      </c>
-      <c r="C6" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="19"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="3">
         <f>SUM(C6:F6)</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f>B6*G6</f>
@@ -854,168 +920,321 @@
         <f>B6^2*G6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10">
-        <v>3</v>
-      </c>
-      <c r="C7" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.2</v>
-      </c>
+      <c r="K6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="e">
+        <f>C6/C$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="1" t="e">
+        <f t="shared" ref="N6:P7" si="2">D6/D$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="e">
+        <f>C6/$G6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="1" t="e">
+        <f t="shared" ref="U6:V6" si="3">D6/$G6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W6" s="1" t="e">
+        <f>F6/$G6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X6" s="5" t="e">
+        <f>T6*T$5+U6*U$5+V6*V$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G8" si="0">SUM(C7:F7)</f>
-        <v>0.60000000000000009</v>
+        <f t="shared" ref="G7:G8" si="4">SUM(C7:F7)</f>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7:H8" si="1">B7*G7</f>
-        <v>1.8000000000000003</v>
+        <f t="shared" ref="H7:H8" si="5">B7*G7</f>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I7:I8" si="2">B7^2*G7</f>
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="17"/>
+        <f t="shared" ref="I7:I8" si="6">B7^2*G7</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="1">
+        <f t="shared" ref="L7:L8" si="7">B7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="e">
+        <f>C7/C$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="1">
+        <f>B7</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="1" t="e">
+        <f>C7/$G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U7" s="1" t="e">
+        <f t="shared" ref="U7" si="8">D7/$G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V7" s="1" t="e">
+        <f t="shared" ref="V7" si="9">E7/$G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W7" s="1" t="e">
+        <f>F7/$G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X7" s="5" t="e">
+        <f t="shared" ref="X7:X8" si="10">T7*T$5+U7*U$5+V7*V$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="22"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="e">
+        <f>C8/C$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" ref="N8" si="11">D8/D$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="1" t="e">
+        <f t="shared" ref="O8" si="12">E8/E$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="1" t="e">
+        <f t="shared" ref="P8" si="13">F8/F$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" s="22"/>
+      <c r="S8" s="1">
+        <f>B8</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="1" t="e">
+        <f>C8/$G8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U8" s="1" t="e">
+        <f t="shared" ref="U8" si="14">D8/$G8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V8" s="1" t="e">
+        <f t="shared" ref="V8" si="15">E8/$G8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W8" s="1" t="e">
+        <f>F8/$G8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X8" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3">
         <f>SUM(C6:C8)</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
         <f>SUM(D6:D8)</f>
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3">
         <f>SUM(E6:E8)</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:G9" si="3">SUM(F6:F8)</f>
+        <f t="shared" ref="F9:G9" si="16">SUM(F6:F8)</f>
         <v>0</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="5" t="e">
+        <f>$L6*M6+$L7*M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="5" t="e">
+        <f>$L6*N6+$L7*N7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="5" t="e">
+        <f>$L6*O6+$L7*O7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="5" t="e">
+        <f>$L6*P6+$L7*P7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1">
         <f>C9*C5</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <f>D9*D5</f>
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <f>E9*E5</f>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
         <f>F9*F5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1">
         <f>C5^2*C9</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:F11" si="4">D5^2*D9</f>
-        <v>1.4</v>
+        <f t="shared" ref="D11:F11" si="17">D5^2*D9</f>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="4"/>
-        <v>25.6</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5">
         <f>SUM(C10:F10)</f>
-        <v>4.1500000000000004</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5">
         <f>SUM(H6:H8)</f>
-        <v>1.8000000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1">
         <f>SUM(C11:F11)</f>
-        <v>27.25</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1">
         <f>SUM(I6:I8)</f>
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5">
         <f>C15-C14^2</f>
-        <v>10.027499999999996</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="5">
         <f>F15-F14^2</f>
-        <v>2.1599999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -1024,14 +1243,14 @@
       </c>
       <c r="C17" s="5">
         <f>SQRT(C16)</f>
-        <v>3.1666228067138018</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="5">
         <f>SQRT(F16)</f>
-        <v>1.4696938456699067</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
@@ -1040,18 +1259,18 @@
       </c>
       <c r="C18" s="1">
         <f>C5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ref="D18:F18" si="5">D5</f>
-        <v>2</v>
+        <f t="shared" ref="D18:F18" si="18">D5</f>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1065,43 +1284,43 @@
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:F21" si="6">D6*D$5*$B6</f>
+        <f t="shared" ref="D19:F21" si="19">D6*D$5*$B6</f>
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
-        <f t="shared" ref="B20:B21" si="7">B7</f>
-        <v>3</v>
+        <f t="shared" ref="B20:B21" si="20">B7</f>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <f>C7*C$5*$B7</f>
-        <v>0.44999999999999996</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="6"/>
-        <v>4.8000000000000007</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="C21" s="1">
@@ -1109,15 +1328,15 @@
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -1127,7 +1346,7 @@
       </c>
       <c r="C23" s="1">
         <f>SUM(C19:F21)</f>
-        <v>6.7500000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
@@ -1136,20 +1355,27 @@
       </c>
       <c r="C24" s="5">
         <f>C23-C14*F14</f>
-        <v>-0.72000000000000064</v>
+        <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="5" t="e">
         <f>C24/SQRT(C16*F16)</f>
-        <v>-0.15470675810139611</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="R6:R8"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="A6:A8"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="T4:W4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Now properly uploading new version
</commit_message>
<xml_diff>
--- a/Exam_prep/Prob_XY.xlsx
+++ b/Exam_prep/Prob_XY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Data Science\Risk Analysis\risk_analysis\Exam_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E1744B-A539-4021-B057-C4455CF86C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133DB18B-00E0-446D-B741-DB929E42BFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Enter your values here:</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>E(Z|Y)</t>
+  </si>
+  <si>
+    <t>This time we even have Conditional Probability:</t>
+  </si>
+  <si>
+    <t>And for exam 190924 problem 5:</t>
+  </si>
+  <si>
+    <t>E(Z|y=2)</t>
+  </si>
+  <si>
+    <t>And you can add more rows and columns in general if a problem wants it:</t>
+  </si>
+  <si>
+    <t>Still works!</t>
   </si>
 </sst>
 </file>
@@ -495,7 +510,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -504,13 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Anteckning" xfId="4" builtinId="10"/>
@@ -798,7 +813,7 @@
   <dimension ref="A4:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F8"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,33 +835,39 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
       <c r="K4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="20"/>
-      <c r="T4" s="18" t="s">
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="23"/>
+      <c r="T4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="20"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
     </row>
     <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="C5" s="17">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="9" t="s">
         <v>4</v>
@@ -862,15 +883,15 @@
       </c>
       <c r="M5" s="1">
         <f>C$5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" ref="N5:P5" si="0">D$5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="0"/>
@@ -881,15 +902,15 @@
       </c>
       <c r="T5" s="1">
         <f>C5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:W5" si="1">D5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V5" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W5" s="1">
         <f t="shared" si="1"/>
@@ -900,207 +921,231 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="B6" s="16">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.3</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="3">
         <f>SUM(C6:F6)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="1">
         <f>B6*G6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
         <f>B6^2*G6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="1">
         <f>B6</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="e">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1">
         <f>C6/C$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="1" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="N6" s="1">
         <f t="shared" ref="N6:P7" si="2">D6/D$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="1" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="P6" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="S6" s="1">
         <f>B6</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="1" t="e">
+        <v>2</v>
+      </c>
+      <c r="T6" s="1">
         <f>C6/$G6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" s="1" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="U6" s="1">
         <f t="shared" ref="U6:V6" si="3">D6/$G6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V6" s="1" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="V6" s="1">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W6" s="1" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="W6" s="1">
         <f>F6/$G6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X6" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="X6" s="5">
         <f>T6*T$5+U6*U$5+V6*V$5</f>
-        <v>#DIV/0!</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.2</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="3">
         <f t="shared" ref="G7:G8" si="4">SUM(C7:F7)</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H8" si="5">B7*G7</f>
-        <v>0</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ref="I7:I8" si="6">B7^2*G7</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="21"/>
+        <v>3.6</v>
+      </c>
+      <c r="K7" s="20"/>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L8" si="7">B7</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="e">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
         <f>C7/C$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="1" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="1" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="P7" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R7" s="21"/>
+      <c r="R7" s="20"/>
       <c r="S7" s="1">
         <f>B7</f>
-        <v>0</v>
-      </c>
-      <c r="T7" s="1" t="e">
+        <v>3</v>
+      </c>
+      <c r="T7" s="1">
         <f>C7/$G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U7" s="1" t="e">
+        <v>0.125</v>
+      </c>
+      <c r="U7" s="1">
         <f t="shared" ref="U7" si="8">D7/$G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V7" s="1" t="e">
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="V7" s="1">
         <f t="shared" ref="V7" si="9">E7/$G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W7" s="1" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="W7" s="1">
         <f>F7/$G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X7" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="X7" s="5">
         <f t="shared" ref="X7:X8" si="10">T7*T$5+U7*U$5+V7*V$5</f>
-        <v>#DIV/0!</v>
+        <v>2.375</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="22"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="22"/>
+        <v>1.6</v>
+      </c>
+      <c r="K8" s="21"/>
       <c r="L8" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="e">
+        <v>4</v>
+      </c>
+      <c r="M8" s="1">
         <f>C8/C$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="1" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" ref="N8" si="11">D8/D$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
         <f t="shared" ref="O8" si="12">E8/E$9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1" t="e">
         <f t="shared" ref="P8" si="13">F8/F$9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R8" s="22"/>
+      <c r="R8" s="21"/>
       <c r="S8" s="1">
         <f>B8</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="1" t="e">
+        <v>4</v>
+      </c>
+      <c r="T8" s="1">
         <f>C8/$G8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" s="1" t="e">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1">
         <f t="shared" ref="U8" si="14">D8/$G8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V8" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
         <f t="shared" ref="V8" si="15">E8/$G8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
         <f>F8/$G8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X8" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="X8" s="5">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
@@ -1109,15 +1154,15 @@
       </c>
       <c r="C9" s="3">
         <f>SUM(C6:C8)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D9" s="3">
         <f>SUM(D6:D8)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E9" s="3">
         <f>SUM(E6:E8)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ref="F9:G9" si="16">SUM(F6:F8)</f>
@@ -1125,22 +1170,22 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="5" t="e">
+      <c r="M9" s="5">
         <f>$L6*M6+$L7*M7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="5" t="e">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="N9" s="5">
         <f>$L6*N6+$L7*N7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="5" t="e">
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="O9" s="5">
         <f>$L6*O6+$L7*O7</f>
-        <v>#DIV/0!</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="P9" s="5" t="e">
         <f>$L6*P6+$L7*P7</f>
@@ -1153,15 +1198,15 @@
       </c>
       <c r="C10" s="1">
         <f>C9*C5</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D10" s="1">
         <f>D9*D5</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="1">
         <f>E9*E5</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F10" s="1">
         <f>F9*F5</f>
@@ -1174,15 +1219,15 @@
       </c>
       <c r="C11" s="1">
         <f>C5^2*C9</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:F11" si="17">D5^2*D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="17"/>
@@ -1195,14 +1240,17 @@
       </c>
       <c r="C14" s="5">
         <f>SUM(C10:F10)</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5">
         <f>SUM(H6:H8)</f>
-        <v>0</v>
+        <v>2.6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
@@ -1211,14 +1259,14 @@
       </c>
       <c r="C15" s="1">
         <f>SUM(C11:F11)</f>
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1">
         <f>SUM(I6:I8)</f>
-        <v>0</v>
+        <v>7.1999999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
@@ -1227,105 +1275,121 @@
       </c>
       <c r="C16" s="5">
         <f>C15-C14^2</f>
-        <v>0</v>
+        <v>0.6875</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="5">
         <f>F15-F14^2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+        <v>0.43999999999999861</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="5">
         <f>SQRT(C16)</f>
-        <v>0</v>
+        <v>0.82915619758884995</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="5">
         <f>SQRT(F16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+        <v>0.66332495807107894</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17">
+        <f>X6</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <f>C5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" ref="D18:F18" si="18">D5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <f>B6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1">
         <f>C6*C$5*$B6</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" ref="D19:F21" si="19">D6*D$5*$B6</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <f t="shared" ref="B20:B21" si="20">B7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1">
         <f>C7*C$5*$B7</f>
-        <v>0</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.8000000000000003</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
         <f>C8*C$5*$B8</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="19"/>
@@ -1340,42 +1404,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="1">
         <f>SUM(C19:F21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="5">
         <f>C23-C14*F14</f>
-        <v>0</v>
+        <v>-0.20000000000000018</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="5" t="e">
+      <c r="F24" s="5">
         <f>C24/SQRT(C16*F16)</f>
-        <v>#DIV/0!</v>
+        <v>-0.36363636363636453</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D35" s="23"/>
+      <c r="D35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T4:W4"/>
     <mergeCell ref="R6:R8"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="K6:K8"/>
-    <mergeCell ref="T4:W4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>